<commit_message>
Restful & To do list update
</commit_message>
<xml_diff>
--- a/ToDo List.xlsx
+++ b/ToDo List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>To do</t>
   </si>
@@ -117,6 +117,27 @@
   </si>
   <si>
     <t>Test with all  browsers</t>
+  </si>
+  <si>
+    <t>Sort timestamp issue</t>
+  </si>
+  <si>
+    <t>Fix buttons on random page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Put scrollbar on divs where needed </t>
+  </si>
+  <si>
+    <t>Email Andy and Ortho</t>
+  </si>
+  <si>
+    <t>Admin adding events ? (possibly)</t>
+  </si>
+  <si>
+    <t>Deletes - Delete messages etc ? (possibly)</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -434,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,26 +478,41 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -523,79 +559,121 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cql statements and testing
</commit_message>
<xml_diff>
--- a/ToDo List.xlsx
+++ b/ToDo List.xlsx
@@ -163,7 +163,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,12 +194,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -213,13 +207,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -493,7 +486,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -504,7 +497,7 @@
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A2" activeCellId="1" sqref="A36 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -561,7 +554,7 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -632,7 +625,7 @@
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -730,7 +723,7 @@
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -740,12 +733,12 @@
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="5" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>